<commit_message>
update vertion AI moquito
</commit_message>
<xml_diff>
--- a/Ngô Trọng Hiếu_22211TT0999_AI muỗi_Version0.0.1-20240503.xlsx
+++ b/Ngô Trọng Hiếu_22211TT0999_AI muỗi_Version0.0.1-20240503.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2023-2024 TDC\SoftwareTesting\Ngô Trọng Hiếu_22211TT0999_Đồ Án_Test Case_Defect List_MindMap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GItTest_2025\Ngô Trọng Hiếu_22211TT0999_Đồ Án_Test Case_Defect List_MindMap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA8D38D-D31D-48B6-A6BB-F281A3D51243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B19120-EEBC-4E22-866E-64A4BFEEC5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E1679A81-637D-4D7F-8787-FADA76073BB0}"/>
   </bookViews>
@@ -35,8 +35,50 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="3">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="3">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="60">
   <si>
     <t>DF_1</t>
   </si>
@@ -133,9 +175,6 @@
     <t>kiểm tra upload file ảnh</t>
   </si>
   <si>
-    <t>B4:Nhận diện loại muỗi và  đưa ra mức độ tương ứng</t>
-  </si>
-  <si>
     <t>B4:không nhận file link ảnh:hiển thị thông báo: No mosquito found</t>
   </si>
   <si>
@@ -150,9 +189,6 @@
 B3:Bấm Up load</t>
   </si>
   <si>
-    <t>B4:Chương trình hiển thị loại muỗi  và độ tin cậy cỉa loại muỗi của con muỗi trong file</t>
-  </si>
-  <si>
     <t>B4:Hiển thị đang load ảnh</t>
   </si>
   <si>
@@ -168,12 +204,6 @@
     <t>Đưa hình anh chibi,meme….</t>
   </si>
   <si>
-    <t>B4:không hiển thị được loại muỗi này</t>
-  </si>
-  <si>
-    <t>B4:vẫn nhận diện được 1 số hình ảnh</t>
-  </si>
-  <si>
     <t>NORMAL</t>
   </si>
   <si>
@@ -193,13 +223,52 @@
   </si>
   <si>
     <t>Version</t>
+  </si>
+  <si>
+    <t>B3:Nhận diện loại muỗi và  đưa ra mức độ tương ứng</t>
+  </si>
+  <si>
+    <t>B2:không hiển thị được loại muỗi này</t>
+  </si>
+  <si>
+    <t>B3:vẫn nhận diện được 1 số hình ảnh</t>
+  </si>
+  <si>
+    <t>B3:Chương trình hiển thị loại muỗi  và độ tin cậy cỉa loại muỗi của con muỗi trong file</t>
+  </si>
+  <si>
+    <t>Cra_2</t>
+  </si>
+  <si>
+    <t>Cra_3</t>
+  </si>
+  <si>
+    <t>Cra_4</t>
+  </si>
+  <si>
+    <t>Cra_5</t>
+  </si>
+  <si>
+    <t>Cra_6</t>
+  </si>
+  <si>
+    <t>Cra_7</t>
+  </si>
+  <si>
+    <t>Cra_8</t>
+  </si>
+  <si>
+    <t>Cra_9</t>
+  </si>
+  <si>
+    <t>Cra_10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +289,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -235,7 +310,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -265,55 +340,27 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -589,6 +636,80 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -908,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F6D6AC-5E66-4925-BC2C-9AF435F6D92B}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="152" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -960,7 +1081,7 @@
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -977,408 +1098,405 @@
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:13" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="6">
+        <v>38051</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="M3" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="I3" s="8">
-        <v>38051</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="91" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="6">
+        <v>38051</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="8">
-        <v>38051</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6" t="s">
-        <v>49</v>
+      <c r="M4" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="6">
+        <v>38051</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="8">
-        <v>38051</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6" t="s">
-        <v>49</v>
+      <c r="M5" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="6">
+        <v>38051</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="8">
-        <v>38051</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6" t="s">
-        <v>49</v>
+      <c r="M6" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="82" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="6">
+        <v>38051</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="8">
-        <v>38051</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6" t="s">
-        <v>49</v>
+      <c r="M7" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="98.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="6">
+        <v>38051</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="8">
-        <v>38051</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6" t="s">
-        <v>49</v>
+      <c r="M8" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="6">
+        <v>38051</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="8">
-        <v>38051</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6" t="s">
-        <v>49</v>
+      <c r="M9" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="6">
+        <v>38051</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="8">
-        <v>38051</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6" t="s">
-        <v>49</v>
+      <c r="M10" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6" t="s">
+      <c r="A11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="5" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="6" t="s">
+      <c r="E11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="6">
+        <v>38051</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="8">
-        <v>38051</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6" t="s">
-        <v>49</v>
+      <c r="M11" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="5" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="I12" s="6">
+        <v>38051</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="6" t="s">
+      <c r="K12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="8">
-        <v>38051</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+      <c r="M12" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>